<commit_message>
After Excel add only
</commit_message>
<xml_diff>
--- a/Excel/Excel.xlsx
+++ b/Excel/Excel.xlsx
@@ -3,21 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\LTI-Eclipse Workspace\easeMyTripDemo1\Excel\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A036ADA-FFB5-4752-A3D0-04B4BFCED13F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{C1ECD6F2-5464-40C1-9E0F-EF5980A80080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="20760" windowHeight="11820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>EmailID</t>
   </si>
@@ -41,13 +37,40 @@
     <t>Contact Number</t>
   </si>
   <si>
-    <t>abc@gmail.com</t>
-  </si>
-  <si>
     <t>Harry</t>
   </si>
   <si>
     <t>Potter</t>
+  </si>
+  <si>
+    <t>CiscoRamon@gmail.com</t>
+  </si>
+  <si>
+    <t>Ramon</t>
+  </si>
+  <si>
+    <t>Cisco</t>
+  </si>
+  <si>
+    <t>HarryPotter@gmail.com</t>
+  </si>
+  <si>
+    <t>HansZimmer@yahoo.com</t>
+  </si>
+  <si>
+    <t>Hans</t>
+  </si>
+  <si>
+    <t>Zimmer</t>
+  </si>
+  <si>
+    <t>9885562171</t>
+  </si>
+  <si>
+    <t>9988556644</t>
+  </si>
+  <si>
+    <t>8774455666</t>
   </si>
 </sst>
 </file>
@@ -92,9 +115,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -376,16 +400,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="17.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25" customWidth="1"/>
+    <col min="2" max="2" width="21.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -399,27 +424,57 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2">
-        <v>9885562171</v>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{339F939B-F9A9-410F-A7CF-842802960A84}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{111B987A-240A-47E7-A234-4674A0F82D8C}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{3534CE59-3CB5-4871-B102-33929464B79C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>